<commit_message>
Push dari kantor udah 90%
</commit_message>
<xml_diff>
--- a/assets/excel/TEMPLATE_SUMMER.xlsx
+++ b/assets/excel/TEMPLATE_SUMMER.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ParTel-Presensi\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F0C320-EE08-4726-A7F4-D3D012550734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480A9926-5EDA-45BA-B48F-E2C84ACAADD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6060FA23-18D8-4869-862B-8C769A129050}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{6060FA23-18D8-4869-862B-8C769A129050}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -456,20 +456,20 @@
   <dimension ref="A1:G175"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,7 +492,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -501,7 +501,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -510,7 +510,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -519,7 +519,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -528,7 +528,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -537,7 +537,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -546,7 +546,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -555,7 +555,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -564,7 +564,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -573,7 +573,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -582,7 +582,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -591,7 +591,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -600,7 +600,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -609,7 +609,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -618,7 +618,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -627,7 +627,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -636,7 +636,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -645,7 +645,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -654,7 +654,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -663,7 +663,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -672,7 +672,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -681,7 +681,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -690,7 +690,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -699,7 +699,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -708,7 +708,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -717,7 +717,7 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -726,7 +726,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -735,7 +735,7 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -744,7 +744,7 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -753,7 +753,7 @@
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -762,7 +762,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -771,7 +771,7 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -780,7 +780,7 @@
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -789,7 +789,7 @@
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -798,7 +798,7 @@
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -807,7 +807,7 @@
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -816,7 +816,7 @@
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -825,7 +825,7 @@
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -834,7 +834,7 @@
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -843,7 +843,7 @@
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -852,7 +852,7 @@
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -861,7 +861,7 @@
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -870,7 +870,7 @@
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -879,7 +879,7 @@
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -888,7 +888,7 @@
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -897,7 +897,7 @@
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -906,7 +906,7 @@
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -915,7 +915,7 @@
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -924,647 +924,650 @@
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D55" s="2"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D56" s="2"/>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D57" s="2"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D58" s="2"/>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D59" s="2"/>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
     </row>
-    <row r="65" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
     </row>
-    <row r="66" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D66" s="2"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
     </row>
-    <row r="67" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D67" s="2"/>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
     </row>
-    <row r="68" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D68" s="2"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
     </row>
-    <row r="69" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D69" s="2"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
     </row>
-    <row r="70" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D70" s="2"/>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
     </row>
-    <row r="71" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D71" s="2"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
     </row>
-    <row r="72" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
     </row>
-    <row r="73" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D73" s="2"/>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
     </row>
-    <row r="74" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D74" s="2"/>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
     </row>
-    <row r="75" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D75" s="2"/>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
     </row>
-    <row r="76" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D76" s="2"/>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
     </row>
-    <row r="77" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D77" s="2"/>
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
     </row>
-    <row r="78" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D78" s="2"/>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
     </row>
-    <row r="79" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D79" s="2"/>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
     </row>
-    <row r="80" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D80" s="2"/>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
     </row>
-    <row r="81" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D81" s="2"/>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
     </row>
-    <row r="82" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D82" s="2"/>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
     </row>
-    <row r="83" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D83" s="2"/>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
     </row>
-    <row r="84" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D84" s="2"/>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
     </row>
-    <row r="85" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D85" s="2"/>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
     </row>
-    <row r="86" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D86" s="2"/>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
     </row>
-    <row r="87" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D87" s="2"/>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
     </row>
-    <row r="88" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D88" s="2"/>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
     </row>
-    <row r="89" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D89" s="2"/>
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
     </row>
-    <row r="90" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D90" s="2"/>
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
     </row>
-    <row r="91" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D91" s="2"/>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
     </row>
-    <row r="92" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D92" s="2"/>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
     </row>
-    <row r="93" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D93" s="2"/>
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
     </row>
-    <row r="94" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D94" s="2"/>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
     </row>
-    <row r="95" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D95" s="2"/>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
     </row>
-    <row r="96" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D96" s="2"/>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
     </row>
-    <row r="97" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D97" s="2"/>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
     </row>
-    <row r="98" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D98" s="2"/>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
     </row>
-    <row r="99" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D99" s="2"/>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
     </row>
-    <row r="100" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D100" s="2"/>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
     </row>
-    <row r="101" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D101" s="2"/>
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
     </row>
-    <row r="102" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="102" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D102" s="2"/>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
     </row>
-    <row r="103" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="103" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D103" s="2"/>
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
     </row>
-    <row r="104" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D104" s="2"/>
       <c r="F104" s="2"/>
       <c r="G104" s="2"/>
     </row>
-    <row r="105" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D105" s="2"/>
       <c r="F105" s="2"/>
       <c r="G105" s="2"/>
     </row>
-    <row r="106" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="106" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D106" s="2"/>
       <c r="F106" s="2"/>
       <c r="G106" s="2"/>
     </row>
-    <row r="107" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="107" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D107" s="2"/>
       <c r="F107" s="2"/>
       <c r="G107" s="2"/>
     </row>
-    <row r="108" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="108" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D108" s="2"/>
       <c r="F108" s="2"/>
       <c r="G108" s="2"/>
     </row>
-    <row r="109" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="109" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D109" s="2"/>
       <c r="F109" s="2"/>
       <c r="G109" s="2"/>
     </row>
-    <row r="110" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="110" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D110" s="2"/>
       <c r="F110" s="2"/>
       <c r="G110" s="2"/>
     </row>
-    <row r="111" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="111" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D111" s="2"/>
       <c r="F111" s="2"/>
       <c r="G111" s="2"/>
     </row>
-    <row r="112" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="112" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D112" s="2"/>
       <c r="F112" s="2"/>
       <c r="G112" s="2"/>
     </row>
-    <row r="113" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="113" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D113" s="2"/>
       <c r="F113" s="2"/>
       <c r="G113" s="2"/>
     </row>
-    <row r="114" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="114" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D114" s="2"/>
       <c r="F114" s="2"/>
       <c r="G114" s="2"/>
     </row>
-    <row r="115" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D115" s="2"/>
       <c r="F115" s="2"/>
       <c r="G115" s="2"/>
     </row>
-    <row r="116" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="116" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D116" s="2"/>
       <c r="F116" s="2"/>
       <c r="G116" s="2"/>
     </row>
-    <row r="117" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="117" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D117" s="2"/>
       <c r="F117" s="2"/>
       <c r="G117" s="2"/>
     </row>
-    <row r="118" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="118" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D118" s="2"/>
       <c r="F118" s="2"/>
       <c r="G118" s="2"/>
     </row>
-    <row r="119" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="119" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D119" s="2"/>
       <c r="F119" s="2"/>
       <c r="G119" s="2"/>
     </row>
-    <row r="120" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="120" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D120" s="2"/>
       <c r="F120" s="2"/>
       <c r="G120" s="2"/>
     </row>
-    <row r="121" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="121" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D121" s="2"/>
       <c r="F121" s="2"/>
       <c r="G121" s="2"/>
     </row>
-    <row r="122" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="122" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D122" s="2"/>
       <c r="F122" s="2"/>
       <c r="G122" s="2"/>
     </row>
-    <row r="123" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="123" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D123" s="2"/>
       <c r="F123" s="2"/>
       <c r="G123" s="2"/>
     </row>
-    <row r="124" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="124" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D124" s="2"/>
       <c r="F124" s="2"/>
       <c r="G124" s="2"/>
     </row>
-    <row r="125" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="125" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D125" s="2"/>
       <c r="F125" s="2"/>
       <c r="G125" s="2"/>
     </row>
-    <row r="126" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="126" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D126" s="2"/>
       <c r="F126" s="2"/>
       <c r="G126" s="2"/>
     </row>
-    <row r="127" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="127" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D127" s="2"/>
       <c r="F127" s="2"/>
       <c r="G127" s="2"/>
     </row>
-    <row r="128" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="128" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D128" s="2"/>
       <c r="F128" s="2"/>
       <c r="G128" s="2"/>
     </row>
-    <row r="129" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="129" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D129" s="2"/>
       <c r="F129" s="2"/>
       <c r="G129" s="2"/>
     </row>
-    <row r="130" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="130" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D130" s="2"/>
       <c r="F130" s="2"/>
       <c r="G130" s="2"/>
     </row>
-    <row r="131" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="131" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D131" s="2"/>
       <c r="F131" s="2"/>
       <c r="G131" s="2"/>
     </row>
-    <row r="132" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="132" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D132" s="2"/>
       <c r="F132" s="2"/>
       <c r="G132" s="2"/>
     </row>
-    <row r="133" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="133" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D133" s="2"/>
       <c r="F133" s="2"/>
       <c r="G133" s="2"/>
     </row>
-    <row r="134" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="134" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D134" s="2"/>
       <c r="F134" s="2"/>
       <c r="G134" s="2"/>
     </row>
-    <row r="135" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="135" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D135" s="2"/>
       <c r="F135" s="2"/>
       <c r="G135" s="2"/>
     </row>
-    <row r="136" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="136" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D136" s="2"/>
       <c r="F136" s="2"/>
       <c r="G136" s="2"/>
     </row>
-    <row r="137" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="137" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D137" s="2"/>
       <c r="F137" s="2"/>
       <c r="G137" s="2"/>
     </row>
-    <row r="138" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="138" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D138" s="2"/>
       <c r="F138" s="2"/>
       <c r="G138" s="2"/>
     </row>
-    <row r="139" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="139" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D139" s="2"/>
       <c r="F139" s="2"/>
       <c r="G139" s="2"/>
     </row>
-    <row r="140" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="140" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D140" s="2"/>
       <c r="F140" s="2"/>
       <c r="G140" s="2"/>
     </row>
-    <row r="141" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="141" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D141" s="2"/>
       <c r="F141" s="2"/>
       <c r="G141" s="2"/>
     </row>
-    <row r="142" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="142" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D142" s="2"/>
       <c r="F142" s="2"/>
       <c r="G142" s="2"/>
     </row>
-    <row r="143" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="143" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D143" s="2"/>
       <c r="F143" s="2"/>
       <c r="G143" s="2"/>
     </row>
-    <row r="144" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="144" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D144" s="2"/>
       <c r="F144" s="2"/>
       <c r="G144" s="2"/>
     </row>
-    <row r="145" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="145" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D145" s="2"/>
       <c r="F145" s="2"/>
       <c r="G145" s="2"/>
     </row>
-    <row r="146" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="146" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D146" s="2"/>
       <c r="F146" s="2"/>
       <c r="G146" s="2"/>
     </row>
-    <row r="147" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="147" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D147" s="2"/>
       <c r="F147" s="2"/>
       <c r="G147" s="2"/>
     </row>
-    <row r="148" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="148" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D148" s="2"/>
       <c r="F148" s="2"/>
       <c r="G148" s="2"/>
     </row>
-    <row r="149" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="149" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D149" s="2"/>
       <c r="F149" s="2"/>
       <c r="G149" s="2"/>
     </row>
-    <row r="150" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="150" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D150" s="2"/>
       <c r="F150" s="2"/>
       <c r="G150" s="2"/>
     </row>
-    <row r="151" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="151" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D151" s="2"/>
       <c r="F151" s="2"/>
       <c r="G151" s="2"/>
     </row>
-    <row r="152" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="152" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D152" s="2"/>
       <c r="F152" s="2"/>
       <c r="G152" s="2"/>
     </row>
-    <row r="153" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="153" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D153" s="2"/>
       <c r="F153" s="2"/>
       <c r="G153" s="2"/>
     </row>
-    <row r="154" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="154" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D154" s="2"/>
       <c r="F154" s="2"/>
       <c r="G154" s="2"/>
     </row>
-    <row r="155" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="155" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D155" s="2"/>
       <c r="F155" s="2"/>
       <c r="G155" s="2"/>
     </row>
-    <row r="156" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="156" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D156" s="2"/>
       <c r="F156" s="2"/>
       <c r="G156" s="2"/>
     </row>
-    <row r="157" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="157" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D157" s="2"/>
       <c r="F157" s="2"/>
       <c r="G157" s="2"/>
     </row>
-    <row r="158" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="158" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D158" s="2"/>
       <c r="F158" s="2"/>
       <c r="G158" s="2"/>
     </row>
-    <row r="159" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="159" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D159" s="2"/>
       <c r="F159" s="2"/>
       <c r="G159" s="2"/>
     </row>
-    <row r="160" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="160" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D160" s="2"/>
       <c r="F160" s="2"/>
       <c r="G160" s="2"/>
     </row>
-    <row r="161" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="161" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D161" s="2"/>
       <c r="F161" s="2"/>
       <c r="G161" s="2"/>
     </row>
-    <row r="162" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="162" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D162" s="2"/>
       <c r="F162" s="2"/>
       <c r="G162" s="2"/>
     </row>
-    <row r="163" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="163" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D163" s="2"/>
       <c r="F163" s="2"/>
       <c r="G163" s="2"/>
     </row>
-    <row r="164" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="164" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D164" s="2"/>
       <c r="F164" s="2"/>
       <c r="G164" s="2"/>
     </row>
-    <row r="165" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="165" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D165" s="2"/>
       <c r="F165" s="2"/>
       <c r="G165" s="2"/>
     </row>
-    <row r="166" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="166" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D166" s="2"/>
       <c r="F166" s="2"/>
       <c r="G166" s="2"/>
     </row>
-    <row r="167" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="167" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D167" s="2"/>
       <c r="F167" s="2"/>
       <c r="G167" s="2"/>
     </row>
-    <row r="168" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="168" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D168" s="2"/>
       <c r="F168" s="2"/>
       <c r="G168" s="2"/>
     </row>
-    <row r="169" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="169" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D169" s="2"/>
       <c r="F169" s="2"/>
       <c r="G169" s="2"/>
     </row>
-    <row r="170" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="170" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D170" s="2"/>
       <c r="F170" s="2"/>
       <c r="G170" s="2"/>
     </row>
-    <row r="171" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="171" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D171" s="2"/>
       <c r="F171" s="2"/>
       <c r="G171" s="2"/>
     </row>
-    <row r="172" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="172" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D172" s="2"/>
       <c r="F172" s="2"/>
       <c r="G172" s="2"/>
     </row>
-    <row r="173" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="173" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D173" s="2"/>
       <c r="F173" s="2"/>
       <c r="G173" s="2"/>
     </row>
-    <row r="174" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="174" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D174" s="2"/>
       <c r="F174" s="2"/>
       <c r="G174" s="2"/>
     </row>
-    <row r="175" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="175" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D175" s="2"/>
       <c r="F175" s="2"/>
       <c r="G175" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G175" xr:uid="{9D67DA94-8760-4304-93C2-3CB6C6A77BC6}">
       <formula1>"SISWA,GURU,-"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F175" xr:uid="{688D9E4D-76FE-47F4-A5E6-E4143641A193}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F175" xr:uid="{688D9E4D-76FE-47F4-A5E6-E4143641A193}">
       <formula1>"BIS-1,BIS-2,BIS-3,BIS-4,-"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D175" xr:uid="{37566B33-1058-49E3-BE58-72BA4D5E0EFF}">
       <formula1>"X-ULW,X-PH,X-KUL-1,X-KUL-2,X-KUL-3,XI-PAR,-"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{728CA371-935D-4507-AC40-374FAD7ADD22}">
+      <formula1>"BUS-1,BUS-2,BUS-3,BUS-4,-"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>